<commit_message>
switched to command pattern
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyt\projekte\scrum_timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38282490-435B-4A31-A0D0-2FF1BB7ECA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D881A9-E022-40C2-B2AF-20DCD1B178C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{A88E9984-2608-4013-A3BE-09F144C42048}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,7 +516,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>44535</v>
+        <v>44545</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
sprints know what itmes they got
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyt\projekte\scrum_timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D881A9-E022-40C2-B2AF-20DCD1B178C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C30849E-A4C0-4F3B-AE5A-049F4F77DB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{A88E9984-2608-4013-A3BE-09F144C42048}"/>
+    <workbookView xWindow="4572" yWindow="1140" windowWidth="16560" windowHeight="9420" xr2:uid="{A88E9984-2608-4013-A3BE-09F144C42048}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>44545</v>
+        <v>44547</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>

</xml_diff>